<commit_message>
changed list of Use cases
</commit_message>
<xml_diff>
--- a/Docs/Use-cases/Use case list.xlsx
+++ b/Docs/Use-cases/Use case list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
   <si>
     <t>Use-case ID</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Review Service Order</t>
   </si>
   <si>
-    <t>Modify Customer Accounts</t>
-  </si>
-  <si>
     <t>Placing request</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>SO workflows</t>
   </si>
   <si>
-    <t>Creating SI</t>
-  </si>
-  <si>
     <t>WIND.UC.018</t>
   </si>
   <si>
@@ -150,12 +144,6 @@
     <t>Bill Sending</t>
   </si>
   <si>
-    <t>Modifying Parameters for SI</t>
-  </si>
-  <si>
-    <t>Disconnect for Existing SI</t>
-  </si>
-  <si>
     <t>Creating RI Reports</t>
   </si>
   <si>
@@ -177,9 +165,6 @@
     <t>+</t>
   </si>
   <si>
-    <t xml:space="preserve"> + |-</t>
-  </si>
-  <si>
     <t>What is done?</t>
   </si>
   <si>
@@ -187,13 +172,28 @@
   </si>
   <si>
     <t>combined with WIND.UC.009</t>
+  </si>
+  <si>
+    <t>Creating Service Instance</t>
+  </si>
+  <si>
+    <t>Modifying Parameters for Service Instance</t>
+  </si>
+  <si>
+    <t>Disconnect for Existing Service Instance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + </t>
+  </si>
+  <si>
+    <t>Changing Customer Password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,6 +226,22 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -260,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -270,6 +286,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -618,13 +637,13 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" customWidth="1"/>
     <col min="3" max="3" width="35.28515625" customWidth="1"/>
     <col min="4" max="4" width="27.42578125" customWidth="1"/>
   </cols>
@@ -640,7 +659,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75">
@@ -654,7 +673,7 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75">
@@ -662,13 +681,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75">
@@ -681,16 +700,22 @@
       <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75">
@@ -701,10 +726,10 @@
         <v>16</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75">
@@ -715,38 +740,38 @@
         <v>17</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75">
-      <c r="A8" t="s">
+      <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>55</v>
+      <c r="B8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75">
-      <c r="A9" t="s">
+      <c r="A9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>56</v>
+      <c r="B9" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75">
@@ -754,13 +779,13 @@
         <v>11</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75">
@@ -768,143 +793,167 @@
         <v>12</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75">
       <c r="A12" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75">
       <c r="A13" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75">
       <c r="A14" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75">
       <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75">
+      <c r="A17" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75">
+      <c r="A18" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75">
-      <c r="A17" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="C21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.75">
-      <c r="A18" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="7" t="s">
+      <c r="C22" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.75">
-      <c r="A19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.75">
-      <c r="A20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75">
-      <c r="A21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.75">
-      <c r="A22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>37</v>
+      <c r="D22" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>